<commit_message>
updated keyboard driven approch selenium automation
</commit_message>
<xml_diff>
--- a/src/main/java/com/kbfb/qa/fb_senerioes/fb_keyboad_senerioes.xlsx
+++ b/src/main/java/com/kbfb/qa/fb_senerioes/fb_keyboad_senerioes.xlsx
@@ -57,12 +57,6 @@
     <t>id=pass</t>
   </si>
   <si>
-    <t>id=login</t>
-  </si>
-  <si>
-    <t>enter   url</t>
-  </si>
-  <si>
     <t>sendskeys</t>
   </si>
   <si>
@@ -85,6 +79,12 @@
   </si>
   <si>
     <t>https://www.facebook.com/</t>
+  </si>
+  <si>
+    <t>name=login</t>
+  </si>
+  <si>
+    <t>enter url</t>
   </si>
 </sst>
 </file>
@@ -452,7 +452,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +488,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -499,10 +499,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -513,10 +513,10 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -527,10 +527,10 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -538,13 +538,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -555,7 +555,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>

</xml_diff>